<commit_message>
fix: update best car
</commit_message>
<xml_diff>
--- a/auto/adac/best_car/cars.xlsx
+++ b/auto/adac/best_car/cars.xlsx
@@ -17,8 +17,8 @@
     <sheet name="sixt_like2drive_meinauto" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AP$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AR$75</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AR$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AP$75</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Spec!$A$1:$AP$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Spec!$A$1:$AP$72</definedName>
   </definedNames>
@@ -488,7 +488,7 @@
     <t xml:space="preserve">plugin hybrid</t>
   </si>
   <si>
-    <t xml:space="preserve">Motorbauart</t>
+    <t xml:space="preserve">Einbauposition / Motorbauart (Verbrennungsmotor)</t>
   </si>
   <si>
     <t xml:space="preserve">[ 'Reihe',  'Boxer', 'V-Motor', 'Voll-Hybrid (Otto/Elektro)', 'E-Motor', 'Hybridsynchronmaschine (HSM)', 'Stromerregte Synchronmaschine (SSM)', 'Permanentmagnet-Synchronmaschine (PSM)','Mild-Hybrid (Otto/Elektro)', 'Mild-Hybrid (Diesel/Elektro)', 'PlugIn-Hybrid (Otto/Elektro)']</t>
@@ -1387,12 +1387,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1462,19 +1462,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AR75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3206" ySplit="0" topLeftCell="A49" activePane="topRight" state="split"/>
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
-      <selection pane="topRight" activeCell="F67" activeCellId="0" sqref="F67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3001" ySplit="0" topLeftCell="A8" activePane="topRight" state="split"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topRight" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.9"/>
@@ -1515,7 +1515,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="13.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="14.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="43" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4627,7 +4626,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP75"/>
+  <autoFilter ref="A1:AR75"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4641,7 +4640,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4653,15 +4652,12 @@
       <selection pane="bottomLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6283,7 +6279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6293,10 +6289,9 @@
       <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7027,7 +7022,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7037,10 +7032,7 @@
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7053,7 +7045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7063,10 +7055,7 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -8050,7 +8039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8060,10 +8049,9 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8284,7 +8272,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8294,10 +8282,7 @@
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="0" t="s">

</xml_diff>

<commit_message>
feat: additional features for scoring
</commit_message>
<xml_diff>
--- a/auto/adac/best_car/cars.xlsx
+++ b/auto/adac/best_car/cars.xlsx
@@ -17,10 +17,10 @@
     <sheet name="sixt_like2drive_meinauto" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AR$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AP$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Spec!$A$1:$AP$74</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Spec!$A$1:$AP$72</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AO$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AQ$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Spec!$A$1:$AO$74</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Spec!$A$1:$AO$72</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI33" authorId="0">
+    <comment ref="AH33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK33" authorId="0">
+    <comment ref="AJ33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="295">
   <si>
     <t xml:space="preserve">feature</t>
   </si>
@@ -281,9 +281,6 @@
     <t xml:space="preserve">vw tiguan</t>
   </si>
   <si>
-    <t xml:space="preserve">subaru outback</t>
-  </si>
-  <si>
     <t xml:space="preserve">hyundai tucson</t>
   </si>
   <si>
@@ -326,6 +323,12 @@
     <t xml:space="preserve">tesla </t>
   </si>
   <si>
+    <t xml:space="preserve">cupra leon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cupra Formentor</t>
+  </si>
+  <si>
     <t xml:space="preserve">AEB pedestrian</t>
   </si>
   <si>
@@ -720,6 +723,15 @@
   </si>
   <si>
     <t xml:space="preserve">electric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADAC additional equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klassenübliche Ausstattung nach ADAC-Vorgabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soundprof</t>
   </si>
   <si>
     <t xml:space="preserve">ford</t>
@@ -1466,15 +1478,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR75"/>
+  <dimension ref="A1:AS77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3001" ySplit="0" topLeftCell="A8" activePane="topRight" state="split"/>
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="topRight" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2160" ySplit="0" topLeftCell="A37" activePane="topRight" state="split"/>
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+      <selection pane="topRight" activeCell="C78" activeCellId="0" sqref="C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.9"/>
@@ -1504,17 +1516,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="12.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="12.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="34" style="0" width="14.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="10.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="13.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="13.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="14.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="0" width="10.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="14.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,22 +1658,25 @@
       <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="0" t="s">
         <v>43</v>
+      </c>
+      <c r="AS1" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>2</v>
@@ -1670,19 +1684,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>3</v>
@@ -1690,19 +1704,19 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>4</v>
@@ -1710,19 +1724,19 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>4</v>
@@ -1730,10 +1744,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>5</v>
@@ -1817,19 +1831,19 @@
         <v>0</v>
       </c>
       <c r="AG6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AI6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL6" s="0" t="n">
         <v>0</v>
@@ -1850,24 +1864,27 @@
         <v>0</v>
       </c>
       <c r="AR6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AS6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>5</v>
@@ -1875,19 +1892,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>5</v>
@@ -1895,16 +1912,16 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>5</v>
@@ -1912,19 +1929,19 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>5</v>
@@ -1932,19 +1949,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>6</v>
@@ -1952,19 +1969,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>6</v>
@@ -1972,10 +1989,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>6</v>
@@ -1983,10 +2000,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>7</v>
@@ -1994,10 +2011,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>7</v>
@@ -2005,10 +2022,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>7</v>
@@ -2016,10 +2033,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>7</v>
@@ -2027,10 +2044,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>7</v>
@@ -2038,16 +2055,16 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>7</v>
@@ -2055,19 +2072,19 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>7</v>
@@ -2075,19 +2092,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>8</v>
@@ -2095,10 +2112,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>8</v>
@@ -2182,7 +2199,7 @@
         <v>0</v>
       </c>
       <c r="AG22" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH22" s="0" t="n">
         <v>1</v>
@@ -2197,7 +2214,7 @@
         <v>1</v>
       </c>
       <c r="AL22" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM22" s="0" t="n">
         <v>0</v>
@@ -2206,24 +2223,27 @@
         <v>0</v>
       </c>
       <c r="AO22" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP22" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ22" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AR22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>8</v>
@@ -2342,19 +2362,22 @@
       <c r="AR23" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="AS23" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>10</v>
@@ -2362,10 +2385,10 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>10</v>
@@ -2476,21 +2499,24 @@
         <v>1</v>
       </c>
       <c r="AP25" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ25" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS25" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>10</v>
@@ -2565,57 +2591,60 @@
         <v>113.3</v>
       </c>
       <c r="AD26" s="0" t="n">
-        <v>110</v>
+        <v>109.9</v>
       </c>
       <c r="AE26" s="0" t="n">
-        <v>109.9</v>
+        <v>114.4</v>
       </c>
       <c r="AF26" s="0" t="n">
-        <v>114.4</v>
+        <v>128.6</v>
       </c>
       <c r="AG26" s="0" t="n">
+        <v>135.5</v>
+      </c>
+      <c r="AH26" s="0" t="n">
         <v>128.6</v>
       </c>
-      <c r="AH26" s="0" t="n">
-        <v>135.5</v>
-      </c>
       <c r="AI26" s="0" t="n">
-        <v>128.6</v>
+        <v>123.7</v>
       </c>
       <c r="AJ26" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="AK26" s="0" t="n">
+        <v>120.8</v>
+      </c>
+      <c r="AL26" s="0" t="n">
+        <v>110.4</v>
+      </c>
+      <c r="AM26" s="0" t="n">
+        <v>129.5</v>
+      </c>
+      <c r="AN26" s="0" t="n">
         <v>123.7</v>
       </c>
-      <c r="AK26" s="0" t="n">
-        <v>125</v>
-      </c>
-      <c r="AL26" s="0" t="n">
-        <v>120.8</v>
-      </c>
-      <c r="AM26" s="0" t="n">
-        <v>110.4</v>
-      </c>
-      <c r="AN26" s="0" t="n">
-        <v>129.5</v>
-      </c>
       <c r="AO26" s="0" t="n">
-        <v>123.7</v>
+        <v>118.7</v>
       </c>
       <c r="AP26" s="0" t="n">
-        <v>118.7</v>
+        <v>126.9</v>
       </c>
       <c r="AQ26" s="0" t="n">
-        <v>126.9</v>
+        <v>127</v>
       </c>
       <c r="AR26" s="0" t="n">
-        <v>127</v>
+        <v>129.7</v>
+      </c>
+      <c r="AS26" s="0" t="n">
+        <v>128.9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>3</v>
@@ -2623,16 +2652,16 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="C28" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>5</v>
@@ -2640,16 +2669,16 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>5</v>
@@ -2657,16 +2686,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>5</v>
@@ -2674,16 +2703,16 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>7</v>
@@ -2691,13 +2720,13 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>7</v>
@@ -2705,10 +2734,10 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>8</v>
@@ -2783,57 +2812,60 @@
         <v>78</v>
       </c>
       <c r="AD33" s="0" t="n">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="AE33" s="0" t="n">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="AF33" s="0" t="n">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="AG33" s="0" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="AH33" s="0" t="n">
         <v>75</v>
       </c>
       <c r="AI33" s="0" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AJ33" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="AK33" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="AL33" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="AK33" s="0" t="n">
-        <v>76</v>
-      </c>
-      <c r="AL33" s="0" t="n">
-        <v>78</v>
-      </c>
       <c r="AM33" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="AN33" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="AO33" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="AP33" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="AQ33" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="AR33" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="AN33" s="0" t="n">
-        <v>71</v>
-      </c>
-      <c r="AO33" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="AP33" s="0" t="n">
+      <c r="AS33" s="0" t="n">
         <v>77</v>
-      </c>
-      <c r="AQ33" s="0" t="n">
-        <v>68</v>
-      </c>
-      <c r="AR33" s="0" t="n">
-        <v>82</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>8</v>
@@ -2908,63 +2940,66 @@
         <v>0.67</v>
       </c>
       <c r="AD34" s="0" t="n">
+        <v>0.606597222222222</v>
+      </c>
+      <c r="AE34" s="0" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="AF34" s="0" t="n">
+        <v>0.70533333333</v>
+      </c>
+      <c r="AG34" s="0" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="AH34" s="0" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="AI34" s="0" t="n">
+        <v>0.653846153846154</v>
+      </c>
+      <c r="AJ34" s="0" t="n">
+        <v>0.667846153846154</v>
+      </c>
+      <c r="AK34" s="0" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="AL34" s="0" t="n">
+        <v>0.64875</v>
+      </c>
+      <c r="AM34" s="0" t="n">
+        <v>0.66266666666</v>
+      </c>
+      <c r="AN34" s="0" t="n">
+        <v>0.68266666666</v>
+      </c>
+      <c r="AO34" s="0" t="n">
+        <v>0.709411764705882</v>
+      </c>
+      <c r="AP34" s="0" t="n">
+        <v>0.624871794871795</v>
+      </c>
+      <c r="AQ34" s="0" t="n">
         <v>0.6</v>
-      </c>
-      <c r="AE34" s="0" t="n">
-        <v>0.606597222222222</v>
-      </c>
-      <c r="AF34" s="0" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="AG34" s="0" t="n">
-        <v>0.70533333333</v>
-      </c>
-      <c r="AH34" s="0" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="AI34" s="0" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="AJ34" s="0" t="n">
-        <v>0.653846153846154</v>
-      </c>
-      <c r="AK34" s="0" t="n">
-        <v>0.667846153846154</v>
-      </c>
-      <c r="AL34" s="0" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="AM34" s="0" t="n">
-        <v>0.64875</v>
-      </c>
-      <c r="AN34" s="0" t="n">
-        <v>0.66266666666</v>
-      </c>
-      <c r="AO34" s="0" t="n">
-        <v>0.68266666666</v>
-      </c>
-      <c r="AP34" s="0" t="n">
-        <v>0.709411764705882</v>
-      </c>
-      <c r="AQ34" s="0" t="n">
-        <v>0.624871794871795</v>
       </c>
       <c r="AR34" s="0" t="n">
         <v>0.6</v>
       </c>
+      <c r="AS34" s="0" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>10</v>
@@ -2972,13 +3007,13 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>15</v>
@@ -2986,18 +3021,18 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>2</v>
@@ -3005,10 +3040,10 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>119</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>4</v>
@@ -3083,13 +3118,13 @@
         <v>1</v>
       </c>
       <c r="AD39" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF39" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG39" s="0" t="n">
         <v>0</v>
@@ -3101,19 +3136,19 @@
         <v>0</v>
       </c>
       <c r="AJ39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK39" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL39" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AM39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN39" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO39" s="0" t="n">
         <v>0</v>
@@ -3125,15 +3160,18 @@
         <v>0</v>
       </c>
       <c r="AR39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AS39" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>4</v>
@@ -3211,10 +3249,10 @@
         <v>0</v>
       </c>
       <c r="AE40" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF40" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG40" s="0" t="n">
         <v>0</v>
@@ -3235,10 +3273,10 @@
         <v>0</v>
       </c>
       <c r="AM40" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN40" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO40" s="0" t="n">
         <v>0</v>
@@ -3250,15 +3288,18 @@
         <v>0</v>
       </c>
       <c r="AR40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>5</v>
@@ -3363,33 +3404,36 @@
         <v>0</v>
       </c>
       <c r="AN41" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AP41" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ41" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AR41" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AS41" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>6</v>
@@ -3397,10 +3441,10 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>2</v>
@@ -3408,10 +3452,10 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>126</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>3</v>
@@ -3419,13 +3463,13 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>3</v>
@@ -3433,10 +3477,10 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>4</v>
@@ -3444,16 +3488,16 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>4</v>
@@ -3461,10 +3505,10 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>4</v>
@@ -3542,10 +3586,10 @@
         <v>1</v>
       </c>
       <c r="AE48" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF48" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG48" s="0" t="n">
         <v>1</v>
@@ -3569,10 +3613,10 @@
         <v>1</v>
       </c>
       <c r="AN48" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO48" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP48" s="0" t="n">
         <v>1</v>
@@ -3581,15 +3625,18 @@
         <v>1</v>
       </c>
       <c r="AR48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS48" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>5</v>
@@ -3664,7 +3711,7 @@
         <v>3</v>
       </c>
       <c r="AD49" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AE49" s="0" t="n">
         <v>3</v>
@@ -3673,28 +3720,28 @@
         <v>3</v>
       </c>
       <c r="AG49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI49" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="AH49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI49" s="0" t="n">
-        <v>1</v>
       </c>
       <c r="AJ49" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AK49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL49" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="AL49" s="0" t="n">
-        <v>2</v>
       </c>
       <c r="AM49" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AN49" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AO49" s="0" t="n">
         <v>1</v>
@@ -3706,15 +3753,18 @@
         <v>1</v>
       </c>
       <c r="AR49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS49" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>5</v>
@@ -3722,13 +3772,13 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>6</v>
@@ -3736,10 +3786,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>6</v>
@@ -3817,7 +3867,7 @@
         <v>0</v>
       </c>
       <c r="AE52" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF52" s="0" t="n">
         <v>1</v>
@@ -3847,24 +3897,27 @@
         <v>1</v>
       </c>
       <c r="AO52" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP52" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ52" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AR52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS52" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>7</v>
@@ -3872,10 +3925,10 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>7</v>
@@ -3883,10 +3936,10 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>8</v>
@@ -3961,22 +4014,22 @@
         <v>2</v>
       </c>
       <c r="AD55" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE55" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF55" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG55" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH55" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AI55" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AJ55" s="0" t="n">
         <v>2</v>
@@ -3985,33 +4038,36 @@
         <v>2</v>
       </c>
       <c r="AL55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN55" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="AM55" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN55" s="0" t="n">
-        <v>1</v>
       </c>
       <c r="AO55" s="0" t="n">
         <v>2</v>
       </c>
       <c r="AP55" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ55" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS55" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>8</v>
@@ -4019,10 +4075,10 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>9</v>
@@ -4106,48 +4162,51 @@
         <v>0</v>
       </c>
       <c r="AG57" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AI57" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ57" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AK57" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL57" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM57" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AN57" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AP57" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ57" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR57" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AS57" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>10</v>
@@ -4222,7 +4281,7 @@
         <v>1</v>
       </c>
       <c r="AD58" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE58" s="0" t="n">
         <v>1</v>
@@ -4231,48 +4290,51 @@
         <v>1</v>
       </c>
       <c r="AG58" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH58" s="0" t="n">
         <v>3</v>
       </c>
       <c r="AI58" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ58" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AJ58" s="0" t="n">
+      <c r="AK58" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AK58" s="0" t="n">
+      <c r="AL58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN58" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="AL58" s="0" t="n">
+      <c r="AO58" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AM58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO58" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="AP58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ58" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="AQ58" s="0" t="n">
-        <v>1</v>
       </c>
       <c r="AR58" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="AS58" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>5</v>
@@ -4280,16 +4342,16 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B60" s="0" t="s">
-        <v>145</v>
-      </c>
       <c r="C60" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F60" s="0" t="n">
         <v>6</v>
@@ -4297,16 +4359,16 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F61" s="0" t="n">
         <v>7</v>
@@ -4314,19 +4376,19 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F62" s="0" t="n">
         <v>10</v>
@@ -4334,19 +4396,19 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D63" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B63" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>154</v>
-      </c>
       <c r="E63" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>13</v>
@@ -4354,13 +4416,13 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F64" s="0" t="n">
         <v>10</v>
@@ -4368,13 +4430,13 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>10</v>
@@ -4382,13 +4444,13 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>7</v>
@@ -4396,16 +4458,16 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F67" s="0" t="n">
         <v>10</v>
@@ -4413,16 +4475,16 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F68" s="0" t="n">
         <v>30</v>
@@ -4430,16 +4492,16 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F69" s="0" t="n">
         <v>50</v>
@@ -4447,10 +4509,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F70" s="0" t="n">
         <v>3</v>
@@ -4458,10 +4520,10 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B71" s="0" t="s">
         <v>171</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>170</v>
       </c>
       <c r="F71" s="0" t="n">
         <v>5</v>
@@ -4469,10 +4531,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F72" s="0" t="n">
         <v>5</v>
@@ -4480,10 +4542,10 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F73" s="0" t="n">
         <v>6</v>
@@ -4491,10 +4553,10 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F74" s="0" t="n">
         <v>8</v>
@@ -4578,13 +4640,13 @@
         <v>0</v>
       </c>
       <c r="AG74" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH74" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AI74" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ74" s="0" t="n">
         <v>0</v>
@@ -4599,7 +4661,7 @@
         <v>0</v>
       </c>
       <c r="AN74" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO74" s="0" t="n">
         <v>1</v>
@@ -4608,25 +4670,59 @@
         <v>1</v>
       </c>
       <c r="AQ74" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS74" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F75" s="0" t="n">
         <v>10</v>
       </c>
     </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AR75"/>
+  <autoFilter ref="A1:AO75"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4646,7 +4742,7 @@
   </sheetPr>
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
@@ -4663,39 +4759,39 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="3"/>
       <c r="C1" s="4" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C2" s="7" t="n">
         <v>2</v>
@@ -4739,13 +4835,13 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="L3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>31240</v>
@@ -4780,7 +4876,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>1940</v>
@@ -4815,7 +4911,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>1000</v>
@@ -4850,7 +4946,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>0.18</v>
@@ -4885,7 +4981,7 @@
     </row>
     <row r="8" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C8" s="13" t="n">
         <f aca="false">SUM(C4:C6)</f>
@@ -4930,7 +5026,7 @@
     </row>
     <row r="9" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="12" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">C8*(1-C7)</f>
@@ -5000,10 +5096,10 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C12" s="9" t="n">
         <v>152</v>
@@ -5053,7 +5149,7 @@
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17"/>
       <c r="B14" s="6" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C14" s="9" t="n">
         <v>820</v>
@@ -5089,7 +5185,7 @@
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17"/>
       <c r="B15" s="6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>868</v>
@@ -5138,7 +5234,7 @@
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17"/>
       <c r="B17" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C17" s="15" t="n">
         <f aca="false">C12+SUM(C14:C15)*0.6</f>
@@ -5207,10 +5303,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C20" s="20" t="n">
         <v>341</v>
@@ -5246,7 +5342,7 @@
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C21" s="23" t="n">
         <v>147</v>
@@ -5282,7 +5378,7 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C22" s="23" t="n">
         <f aca="false">C21</f>
@@ -5328,7 +5424,7 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="22" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C23" s="25" t="n">
         <f aca="false">C17/12</f>
@@ -5374,7 +5470,7 @@
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C24" s="27" t="n">
         <v>100</v>
@@ -5410,7 +5506,7 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C25" s="23" t="n">
         <v>81</v>
@@ -5446,7 +5542,7 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C26" s="23" t="n">
         <f aca="false">C25</f>
@@ -5506,7 +5602,7 @@
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="6" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C28" s="9" t="n">
         <f aca="false">SUM(C20:C26)-C24</f>
@@ -5565,7 +5661,7 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="6" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C30" s="15" t="n">
         <f aca="false">C28-C20</f>
@@ -5624,10 +5720,10 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C32" s="9" t="n">
         <f aca="false">C28*12</f>
@@ -5673,7 +5769,7 @@
     <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="29"/>
       <c r="B33" s="30" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C33" s="31" t="n">
         <f aca="false">C32*5</f>
@@ -5719,7 +5815,7 @@
     <row r="34" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="29"/>
       <c r="B34" s="12" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C34" s="13" t="n">
         <f aca="false">C33+C9</f>
@@ -5764,10 +5860,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="29" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C36" s="9" t="n">
         <f aca="false">C30*12</f>
@@ -5813,7 +5909,7 @@
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="29"/>
       <c r="B37" s="30" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C37" s="31" t="n">
         <f aca="false">C36*5</f>
@@ -5859,7 +5955,7 @@
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="29"/>
       <c r="B38" s="12" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C38" s="13" t="n">
         <f aca="false">C37+C9</f>
@@ -5918,7 +6014,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>0.39</v>
@@ -5953,7 +6049,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C41" s="15" t="n">
         <f aca="false">C9*C40</f>
@@ -6010,7 +6106,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C43" s="15" t="n">
         <f aca="false">(C38-C41)/60</f>
@@ -6285,7 +6381,7 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -6296,33 +6392,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B2" s="33" t="n">
         <v>405.65</v>
@@ -6349,7 +6445,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B3" s="33" t="n">
         <v>570.34</v>
@@ -6375,7 +6471,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B4" s="33" t="n">
         <v>684.6</v>
@@ -6401,7 +6497,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B5" s="33" t="n">
         <v>335.21</v>
@@ -6427,7 +6523,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B6" s="33" t="n">
         <v>576.47</v>
@@ -6453,7 +6549,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B7" s="33" t="n">
         <v>190.91</v>
@@ -6479,7 +6575,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B8" s="33" t="n">
         <v>691.18</v>
@@ -6505,7 +6601,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B9" s="33" t="n">
         <v>602.66</v>
@@ -6531,7 +6627,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B10" s="33" t="n">
         <v>320.22</v>
@@ -6557,7 +6653,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="33" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B11" s="33" t="n">
         <v>171.35</v>
@@ -6583,7 +6679,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B12" s="33" t="n">
         <v>43.37</v>
@@ -6609,7 +6705,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>103.67</v>
@@ -6635,7 +6731,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>160.94</v>
@@ -6661,7 +6757,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>125.06</v>
@@ -6687,7 +6783,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="33" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>254.38</v>
@@ -6713,7 +6809,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B17" s="33" t="n">
         <v>341.67</v>
@@ -6739,7 +6835,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="33" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B18" s="33" t="n">
         <v>60.94</v>
@@ -6765,7 +6861,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="33" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B19" s="33" t="n">
         <v>174.61</v>
@@ -6791,7 +6887,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B20" s="33" t="n">
         <v>346.57</v>
@@ -6817,7 +6913,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="33" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B21" s="33" t="n">
         <v>345.27</v>
@@ -6843,7 +6939,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="33" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B22" s="33" t="n">
         <v>238.6</v>
@@ -6869,7 +6965,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="33" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B23" s="33" t="n">
         <v>504.66</v>
@@ -6895,7 +6991,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="33" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B24" s="33" t="n">
         <v>102.7</v>
@@ -6927,7 +7023,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G26" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">H25/23</f>
@@ -6936,7 +7032,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>320</v>
@@ -6947,7 +7043,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>210</v>
@@ -6958,7 +7054,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>87</v>
@@ -6969,7 +7065,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>83</v>
@@ -6980,7 +7076,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>15</v>
@@ -6991,7 +7087,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>12</v>
@@ -7028,11 +7124,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7051,15 +7147,15 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8024,7 +8120,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -8045,35 +8141,35 @@
   </sheetPr>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="34" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C1" s="34"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>36</v>
@@ -8087,7 +8183,7 @@
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -8102,7 +8198,7 @@
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="35" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -8117,7 +8213,7 @@
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="35" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -8132,7 +8228,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -8147,7 +8243,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>325</v>
@@ -8157,7 +8253,7 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>461</v>
@@ -8172,7 +8268,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>4.2</v>
@@ -8183,7 +8279,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -8194,13 +8290,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8278,49 +8374,49 @@
   </sheetPr>
   <dimension ref="A3:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>414</v>
@@ -8344,10 +8440,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">SUM(E6:F6)</f>
@@ -8356,10 +8452,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">SUM(E7:F7)</f>
@@ -8368,16 +8464,16 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>484.9</v>
@@ -8398,16 +8494,16 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>540.33</v>
@@ -8419,16 +8515,16 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>499</v>
@@ -8446,16 +8542,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>378</v>
@@ -8473,16 +8569,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>529</v>
@@ -8500,16 +8596,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>704</v>
@@ -8521,16 +8617,16 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>426.63</v>

</xml_diff>

<commit_message>
fix: removed formatting for empty rows
</commit_message>
<xml_diff>
--- a/auto/adac/best_car/cars.xlsx
+++ b/auto/adac/best_car/cars.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="294">
   <si>
     <t xml:space="preserve">feature</t>
   </si>
@@ -729,9 +729,6 @@
   </si>
   <si>
     <t xml:space="preserve">Klassenübliche Ausstattung nach ADAC-Vorgabe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soundprof</t>
   </si>
   <si>
     <t xml:space="preserve">ford</t>
@@ -1478,20 +1475,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AS77"/>
+  <dimension ref="A1:AS76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2160" ySplit="0" topLeftCell="A37" activePane="topRight" state="split"/>
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
-      <selection pane="topRight" activeCell="C78" activeCellId="0" sqref="C78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1885" ySplit="0" topLeftCell="A55" activePane="topRight" state="split"/>
+      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+      <selection pane="topRight" activeCell="A76" activeCellId="0" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.83"/>
@@ -1679,7 +1677,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,7 +1717,7 @@
         <v>52</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,7 +1737,7 @@
         <v>52</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,7 +1885,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,7 +1905,7 @@
         <v>52</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,7 +1922,7 @@
         <v>63</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,7 +1942,7 @@
         <v>52</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,7 +1962,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1984,7 +1982,7 @@
         <v>52</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,7 +1993,7 @@
         <v>46</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,7 +2004,7 @@
         <v>46</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2017,7 +2015,7 @@
         <v>46</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,7 +2026,7 @@
         <v>46</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2039,7 +2037,7 @@
         <v>46</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,7 +2048,7 @@
         <v>46</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,7 +2065,7 @@
         <v>83</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,7 +2085,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,7 +2105,7 @@
         <v>52</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2118,7 +2116,7 @@
         <v>46</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0</v>
@@ -2246,7 +2244,7 @@
         <v>46</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>1</v>
@@ -2380,7 +2378,7 @@
         <v>93</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2519,7 +2517,7 @@
         <v>46</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>113.3</v>
@@ -2647,7 +2645,7 @@
         <v>97</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2681,7 +2679,7 @@
         <v>103</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2729,7 +2727,7 @@
         <v>111</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2740,7 +2738,7 @@
         <v>97</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>77</v>
@@ -2868,7 +2866,7 @@
         <v>97</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>0.6225</v>
@@ -3035,7 +3033,7 @@
         <v>120</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3046,7 +3044,7 @@
         <v>120</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>0</v>
@@ -3174,7 +3172,7 @@
         <v>120</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>0</v>
@@ -3436,7 +3434,7 @@
         <v>52</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3447,7 +3445,7 @@
         <v>127</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,7 +3456,7 @@
         <v>127</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3470,7 @@
         <v>130</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3483,7 +3481,7 @@
         <v>127</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3500,7 +3498,7 @@
         <v>52</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3511,7 +3509,7 @@
         <v>127</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>0</v>
@@ -3781,7 +3779,7 @@
         <v>138</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,7 +3790,7 @@
         <v>127</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G52" s="0" t="n">
         <v>1</v>
@@ -3920,7 +3918,7 @@
         <v>127</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,7 +3929,7 @@
         <v>127</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3942,7 +3940,7 @@
         <v>127</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G55" s="0" t="n">
         <v>2</v>
@@ -4070,7 +4068,7 @@
         <v>127</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4081,7 +4079,7 @@
         <v>127</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G57" s="0" t="n">
         <v>0</v>
@@ -4354,7 +4352,7 @@
         <v>149</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4371,7 +4369,7 @@
         <v>152</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4391,7 +4389,7 @@
         <v>52</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4411,7 +4409,7 @@
         <v>52</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4425,7 +4423,7 @@
         <v>159</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4439,7 +4437,7 @@
         <v>161</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4453,7 +4451,7 @@
         <v>163</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4515,7 +4513,7 @@
         <v>171</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4526,7 +4524,7 @@
         <v>171</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4548,7 +4546,7 @@
         <v>171</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4559,7 +4557,7 @@
         <v>171</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G74" s="0" t="n">
         <v>1</v>
@@ -4704,21 +4702,7 @@
         <v>52</v>
       </c>
       <c r="F76" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -4759,39 +4743,39 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="3"/>
       <c r="C1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="7" t="n">
         <v>2</v>
@@ -4835,7 +4819,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L3" s="8"/>
     </row>
@@ -4876,7 +4860,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>1940</v>
@@ -4911,7 +4895,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>1000</v>
@@ -4946,7 +4930,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>0.18</v>
@@ -4981,7 +4965,7 @@
     </row>
     <row r="8" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="13" t="n">
         <f aca="false">SUM(C4:C6)</f>
@@ -5026,7 +5010,7 @@
     </row>
     <row r="9" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">C8*(1-C7)</f>
@@ -5096,10 +5080,10 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="C12" s="9" t="n">
         <v>152</v>
@@ -5149,7 +5133,7 @@
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17"/>
       <c r="B14" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C14" s="9" t="n">
         <v>820</v>
@@ -5185,7 +5169,7 @@
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17"/>
       <c r="B15" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" s="9" t="n">
         <v>868</v>
@@ -5234,7 +5218,7 @@
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17"/>
       <c r="B17" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C17" s="15" t="n">
         <f aca="false">C12+SUM(C14:C15)*0.6</f>
@@ -5303,7 +5287,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>165</v>
@@ -5602,7 +5586,7 @@
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28" s="9" t="n">
         <f aca="false">SUM(C20:C26)-C24</f>
@@ -5661,7 +5645,7 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" s="15" t="n">
         <f aca="false">C28-C20</f>
@@ -5720,10 +5704,10 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>205</v>
       </c>
       <c r="C32" s="9" t="n">
         <f aca="false">C28*12</f>
@@ -5769,7 +5753,7 @@
     <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="29"/>
       <c r="B33" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C33" s="31" t="n">
         <f aca="false">C32*5</f>
@@ -5815,7 +5799,7 @@
     <row r="34" s="11" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="29"/>
       <c r="B34" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C34" s="13" t="n">
         <f aca="false">C33+C9</f>
@@ -5860,10 +5844,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C36" s="9" t="n">
         <f aca="false">C30*12</f>
@@ -5909,7 +5893,7 @@
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="29"/>
       <c r="B37" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C37" s="31" t="n">
         <f aca="false">C36*5</f>
@@ -5955,7 +5939,7 @@
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="29"/>
       <c r="B38" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C38" s="13" t="n">
         <f aca="false">C37+C9</f>
@@ -6014,7 +5998,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>0.39</v>
@@ -6049,7 +6033,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C41" s="15" t="n">
         <f aca="false">C9*C40</f>
@@ -6106,7 +6090,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C43" s="15" t="n">
         <f aca="false">(C38-C41)/60</f>
@@ -6392,33 +6376,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>218</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="33" t="n">
         <v>405.65</v>
@@ -6445,7 +6429,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3" s="33" t="n">
         <v>570.34</v>
@@ -6471,7 +6455,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B4" s="33" t="n">
         <v>684.6</v>
@@ -6497,7 +6481,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B5" s="33" t="n">
         <v>335.21</v>
@@ -6523,7 +6507,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B6" s="33" t="n">
         <v>576.47</v>
@@ -6549,7 +6533,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7" s="33" t="n">
         <v>190.91</v>
@@ -6575,7 +6559,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B8" s="33" t="n">
         <v>691.18</v>
@@ -6601,7 +6585,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B9" s="33" t="n">
         <v>602.66</v>
@@ -6627,7 +6611,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B10" s="33" t="n">
         <v>320.22</v>
@@ -6653,7 +6637,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B11" s="33" t="n">
         <v>171.35</v>
@@ -6679,7 +6663,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B12" s="33" t="n">
         <v>43.37</v>
@@ -6705,7 +6689,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" s="33" t="n">
         <v>103.67</v>
@@ -6731,7 +6715,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B14" s="33" t="n">
         <v>160.94</v>
@@ -6757,7 +6741,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B15" s="33" t="n">
         <v>125.06</v>
@@ -6783,7 +6767,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B16" s="33" t="n">
         <v>254.38</v>
@@ -6809,7 +6793,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B17" s="33" t="n">
         <v>341.67</v>
@@ -6835,7 +6819,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B18" s="33" t="n">
         <v>60.94</v>
@@ -6861,7 +6845,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B19" s="33" t="n">
         <v>174.61</v>
@@ -6887,7 +6871,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B20" s="33" t="n">
         <v>346.57</v>
@@ -6913,7 +6897,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B21" s="33" t="n">
         <v>345.27</v>
@@ -6939,7 +6923,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B22" s="33" t="n">
         <v>238.6</v>
@@ -6965,7 +6949,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B23" s="33" t="n">
         <v>504.66</v>
@@ -6991,7 +6975,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B24" s="33" t="n">
         <v>102.7</v>
@@ -7023,7 +7007,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G26" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H26" s="0" t="n">
         <f aca="false">H25/23</f>
@@ -7032,7 +7016,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>320</v>
@@ -7043,7 +7027,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>210</v>
@@ -7054,7 +7038,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>87</v>
@@ -7065,7 +7049,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>83</v>
@@ -7076,7 +7060,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>15</v>
@@ -7087,7 +7071,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>12</v>
@@ -7128,7 +7112,7 @@
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7151,11 +7135,11 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8120,7 +8104,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -8145,31 +8129,31 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C1" s="34"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>36</v>
@@ -8183,7 +8167,7 @@
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -8198,7 +8182,7 @@
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -8213,7 +8197,7 @@
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -8228,7 +8212,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -8243,7 +8227,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>325</v>
@@ -8253,7 +8237,7 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>461</v>
@@ -8268,7 +8252,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>4.2</v>
@@ -8279,7 +8263,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -8290,13 +8274,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>266</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8378,45 +8362,45 @@
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>272</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>414</v>
@@ -8440,10 +8424,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>278</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>279</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">SUM(E6:F6)</f>
@@ -8452,10 +8436,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">SUM(E7:F7)</f>
@@ -8464,16 +8448,16 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>281</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>282</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>484.9</v>
@@ -8494,16 +8478,16 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>284</v>
-      </c>
       <c r="C9" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>540.33</v>
@@ -8515,16 +8499,16 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>286</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>287</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>499</v>
@@ -8542,16 +8526,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>288</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>289</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>378</v>
@@ -8569,16 +8553,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>291</v>
-      </c>
       <c r="C12" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>529</v>
@@ -8596,16 +8580,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>292</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>293</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>704</v>
@@ -8617,16 +8601,16 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>276</v>
-      </c>
       <c r="D14" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>426.63</v>

</xml_diff>

<commit_message>
adac best car update to latest data
</commit_message>
<xml_diff>
--- a/auto/adac/best_car/cars.xlsx
+++ b/auto/adac/best_car/cars.xlsx
@@ -17,8 +17,8 @@
     <sheet name="sixt_like2drive_meinauto" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AO$75</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AQ$75</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AQ$75</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Spec!$A$1:$AO$75</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Spec!$A$1:$AO$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Spec!$A$1:$AO$72</definedName>
   </definedNames>
@@ -665,7 +665,7 @@
     <t xml:space="preserve">Insurance 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Vollkaskobetrag 100% 500 Euro SB</t>
+    <t xml:space="preserve">Vollkaskobetrag 100% 500 € SB</t>
   </si>
   <si>
     <t xml:space="preserve">Costs service</t>
@@ -1477,13 +1477,13 @@
   </sheetPr>
   <dimension ref="A1:AS76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1885" ySplit="0" topLeftCell="A55" activePane="topRight" state="split"/>
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
-      <selection pane="topRight" activeCell="A76" activeCellId="0" sqref="A76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1769" ySplit="0" topLeftCell="A43" activePane="topRight" state="split"/>
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+      <selection pane="topRight" activeCell="C61" activeCellId="0" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.9"/>
@@ -4706,10 +4706,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO75"/>
+  <autoFilter ref="A1:AQ75"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -6349,7 +6349,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7093,7 +7093,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7112,11 +7112,11 @@
       <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -7135,7 +7135,7 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -8110,7 +8110,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -8129,7 +8129,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.13"/>
   </cols>
@@ -8343,7 +8343,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -8362,7 +8362,7 @@
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="0" t="s">
@@ -8623,7 +8623,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>